<commit_message>
updated metadata annotation human excel file
</commit_message>
<xml_diff>
--- a/data/article_metadata_ephys_annotations.xlsx
+++ b/data/article_metadata_ephys_annotations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="1116">
   <si>
     <t>Article title</t>
   </si>
@@ -1797,66 +1797,9 @@
     <t>barrel cortex</t>
   </si>
   <si>
-    <t>mGluR5 in cortical excitatory neurons exerts both cell-autonomous and -nonautonomous influences on cortical somatosensory circuit formation.</t>
-  </si>
-  <si>
-    <t>http://www.jneurosci.org/content/30/50/16896.full</t>
-  </si>
-  <si>
-    <t>Predominance of late-spiking neurons in layer VI of rat perirhinal cortex.</t>
-  </si>
-  <si>
-    <t>http://www.jneurosci.org/content/21/14/4969.full</t>
-  </si>
-  <si>
-    <t>Electrophysiological classes of cat primary visual cortical neurons in vivo as revealed by quantitative analyses.</t>
-  </si>
-  <si>
-    <t>http://jn.physiology.org/content/89/3/1541.full</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cat </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">P14–P20 </t>
   </si>
   <si>
-    <t>Cdk5 modulates cocaine reward, motivation, and striatal neuron excitability.</t>
-  </si>
-  <si>
-    <t>http://www.jneurosci.org/content/27/47/12967.full</t>
-  </si>
-  <si>
-    <t>Nucleus accumbens medium spiny neuron</t>
-  </si>
-  <si>
-    <t>Maturation of excitatory synaptic transmission of the rat nucleus accumbens from juvenile to adult.</t>
-  </si>
-  <si>
-    <t>http://jn.physiology.org/content/101/5/2516.long</t>
-  </si>
-  <si>
-    <t>Exposure to cocaine dynamically regulates the intrinsic membrane excitability of nucleus accumbens neurons.</t>
-  </si>
-  <si>
-    <t>http://www.jneurosci.org/content/30/10/3689.full</t>
-  </si>
-  <si>
-    <t>Nucleus accumbens shell neuron</t>
-  </si>
-  <si>
-    <t>Selective disruption of nucleus accumbens gating mechanisms in rats behaviorally sensitized to methamphetamine.</t>
-  </si>
-  <si>
-    <t>http://www.jneurosci.org/content/25/28/6687.full</t>
-  </si>
-  <si>
-    <t>Nucleus accumbens core neuron</t>
-  </si>
-  <si>
     <t>Hippocampus CA3 basket cell</t>
   </si>
   <si>
@@ -3393,42 +3336,6 @@
     <t>85.9</t>
   </si>
   <si>
-    <t>21159961</t>
-  </si>
-  <si>
-    <t>-60.32</t>
-  </si>
-  <si>
-    <t>128.3</t>
-  </si>
-  <si>
-    <t>8.09</t>
-  </si>
-  <si>
-    <t>76.43</t>
-  </si>
-  <si>
-    <t>-36.91</t>
-  </si>
-  <si>
-    <t>11438572</t>
-  </si>
-  <si>
-    <t>-80.9</t>
-  </si>
-  <si>
-    <t>557</t>
-  </si>
-  <si>
-    <t>102.3</t>
-  </si>
-  <si>
-    <t>86.1</t>
-  </si>
-  <si>
-    <t>12626627</t>
-  </si>
-  <si>
     <t>-67.15</t>
   </si>
   <si>
@@ -3442,60 +3349,6 @@
   </si>
   <si>
     <t>-37.27</t>
-  </si>
-  <si>
-    <t>18032670</t>
-  </si>
-  <si>
-    <t>-81.8</t>
-  </si>
-  <si>
-    <t>72.4</t>
-  </si>
-  <si>
-    <t>-42.8</t>
-  </si>
-  <si>
-    <t>19244354</t>
-  </si>
-  <si>
-    <t>-93.5</t>
-  </si>
-  <si>
-    <t>-46.4</t>
-  </si>
-  <si>
-    <t>20220002</t>
-  </si>
-  <si>
-    <t>-82.55</t>
-  </si>
-  <si>
-    <t>130.4</t>
-  </si>
-  <si>
-    <t>-31.97</t>
-  </si>
-  <si>
-    <t>16014730</t>
-  </si>
-  <si>
-    <t>53.8</t>
-  </si>
-  <si>
-    <t>5.9</t>
-  </si>
-  <si>
-    <t>-48.3</t>
-  </si>
-  <si>
-    <t>85.4</t>
-  </si>
-  <si>
-    <t>5.2</t>
-  </si>
-  <si>
-    <t>-49.7</t>
   </si>
   <si>
     <t>122.9</t>
@@ -3851,10 +3704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S141"/>
+  <dimension ref="A1:S133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3933,7 +3786,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>619</v>
+        <v>600</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>21</v>
@@ -3962,22 +3815,22 @@
         <v>28</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>620</v>
+        <v>601</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>621</v>
+        <v>602</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>622</v>
+        <v>603</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>623</v>
+        <v>604</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>624</v>
+        <v>605</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>625</v>
+        <v>606</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -3988,7 +3841,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>626</v>
+        <v>607</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>21</v>
@@ -4017,22 +3870,22 @@
         <v>28</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>627</v>
+        <v>608</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>628</v>
+        <v>609</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>629</v>
+        <v>610</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>630</v>
+        <v>611</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -4043,7 +3896,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>631</v>
+        <v>612</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>21</v>
@@ -4072,22 +3925,22 @@
         <v>28</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>632</v>
+        <v>613</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>35</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>634</v>
+        <v>615</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>35</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>635</v>
+        <v>616</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -4098,7 +3951,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>636</v>
+        <v>617</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>21</v>
@@ -4127,22 +3980,22 @@
         <v>28</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>637</v>
+        <v>618</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>638</v>
+        <v>619</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>639</v>
+        <v>620</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>640</v>
+        <v>621</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>641</v>
+        <v>622</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -4153,7 +4006,7 @@
         <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>642</v>
+        <v>623</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>21</v>
@@ -4182,19 +4035,19 @@
         <v>28</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>643</v>
+        <v>624</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>644</v>
+        <v>625</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>645</v>
+        <v>626</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>646</v>
+        <v>627</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>647</v>
+        <v>628</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>35</v>
@@ -4208,7 +4061,7 @@
         <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>648</v>
+        <v>629</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>21</v>
@@ -4237,22 +4090,22 @@
         <v>28</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>649</v>
+        <v>630</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>650</v>
+        <v>631</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>651</v>
+        <v>632</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>652</v>
+        <v>633</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>653</v>
+        <v>634</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>654</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -4263,7 +4116,7 @@
         <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>655</v>
+        <v>636</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>21</v>
@@ -4292,7 +4145,7 @@
         <v>28</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>656</v>
+        <v>637</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>35</v>
@@ -4301,7 +4154,7 @@
         <v>35</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>657</v>
+        <v>638</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>35</v>
@@ -4318,7 +4171,7 @@
         <v>58</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>658</v>
+        <v>639</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>21</v>
@@ -4350,19 +4203,19 @@
         <v>35</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>659</v>
+        <v>640</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>660</v>
+        <v>641</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>661</v>
+        <v>642</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -4373,7 +4226,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>662</v>
+        <v>643</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>21</v>
@@ -4390,7 +4243,7 @@
         <v>66</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>663</v>
+        <v>644</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>67</v>
@@ -4402,10 +4255,10 @@
         <v>28</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>664</v>
+        <v>645</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>659</v>
+        <v>640</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>35</v>
@@ -4414,10 +4267,10 @@
         <v>35</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>665</v>
+        <v>646</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>666</v>
+        <v>647</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -4428,7 +4281,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>667</v>
+        <v>648</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
@@ -4457,10 +4310,10 @@
         <v>28</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>668</v>
+        <v>649</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>669</v>
+        <v>650</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>35</v>
@@ -4469,10 +4322,10 @@
         <v>35</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>670</v>
+        <v>651</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>671</v>
+        <v>652</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -4483,7 +4336,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>672</v>
+        <v>653</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>21</v>
@@ -4514,10 +4367,10 @@
         <v>28</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>673</v>
+        <v>654</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>674</v>
+        <v>655</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>35</v>
@@ -4540,7 +4393,7 @@
         <v>81</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>675</v>
+        <v>656</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>21</v>
@@ -4569,10 +4422,10 @@
         <v>28</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>676</v>
+        <v>657</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>677</v>
+        <v>658</v>
       </c>
       <c r="P13" s="2" t="s">
         <v>35</v>
@@ -4595,7 +4448,7 @@
         <v>85</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>678</v>
+        <v>659</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>21</v>
@@ -4624,22 +4477,22 @@
         <v>28</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>679</v>
+        <v>660</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>681</v>
+        <v>662</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>682</v>
+        <v>663</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>683</v>
+        <v>664</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -4650,7 +4503,7 @@
         <v>89</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>684</v>
+        <v>665</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>21</v>
@@ -4679,19 +4532,19 @@
         <v>28</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>685</v>
+        <v>666</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>686</v>
+        <v>667</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>687</v>
+        <v>668</v>
       </c>
       <c r="Q15" s="2" t="s">
         <v>35</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>688</v>
+        <v>669</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>35</v>
@@ -4705,7 +4558,7 @@
         <v>94</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>689</v>
+        <v>670</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>21</v>
@@ -4762,7 +4615,7 @@
         <v>99</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>690</v>
+        <v>671</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>21</v>
@@ -4791,10 +4644,10 @@
         <v>28</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>691</v>
+        <v>672</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>692</v>
+        <v>673</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>35</v>
@@ -4806,7 +4659,7 @@
         <v>35</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>693</v>
+        <v>674</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -4817,7 +4670,7 @@
         <v>105</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>694</v>
+        <v>675</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>21</v>
@@ -4848,13 +4701,13 @@
         <v>28</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>695</v>
+        <v>676</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>696</v>
+        <v>677</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>697</v>
+        <v>678</v>
       </c>
       <c r="Q18" s="2" t="s">
         <v>35</v>
@@ -4874,7 +4727,7 @@
         <v>111</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>698</v>
+        <v>679</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>21</v>
@@ -4903,22 +4756,22 @@
         <v>28</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>699</v>
+        <v>680</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>700</v>
+        <v>681</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>35</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>701</v>
+        <v>682</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>35</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>702</v>
+        <v>683</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -4929,7 +4782,7 @@
         <v>117</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>703</v>
+        <v>684</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>21</v>
@@ -4958,10 +4811,10 @@
         <v>28</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>704</v>
+        <v>685</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>705</v>
+        <v>686</v>
       </c>
       <c r="P20" s="2" t="s">
         <v>35</v>
@@ -4984,7 +4837,7 @@
         <v>121</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>706</v>
+        <v>687</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>21</v>
@@ -5013,22 +4866,22 @@
         <v>28</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>707</v>
+        <v>688</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>708</v>
+        <v>689</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>35</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>709</v>
+        <v>690</v>
       </c>
       <c r="R21" s="2" t="s">
         <v>35</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>710</v>
+        <v>691</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -5039,7 +4892,7 @@
         <v>125</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>711</v>
+        <v>692</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>21</v>
@@ -5068,16 +4921,16 @@
         <v>28</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>643</v>
+        <v>624</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>712</v>
+        <v>693</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>713</v>
+        <v>694</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>35</v>
@@ -5094,7 +4947,7 @@
         <v>129</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>714</v>
+        <v>695</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>21</v>
@@ -5123,10 +4976,10 @@
         <v>28</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>715</v>
+        <v>696</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>716</v>
+        <v>697</v>
       </c>
       <c r="P23" s="2" t="s">
         <v>35</v>
@@ -5149,7 +5002,7 @@
         <v>134</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>717</v>
+        <v>698</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>21</v>
@@ -5178,22 +5031,22 @@
         <v>28</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>718</v>
+        <v>699</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>719</v>
+        <v>700</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>720</v>
+        <v>701</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>721</v>
+        <v>702</v>
       </c>
       <c r="R24" s="2" t="s">
         <v>35</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>722</v>
+        <v>703</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -5204,7 +5057,7 @@
         <v>137</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>723</v>
+        <v>704</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>21</v>
@@ -5233,22 +5086,22 @@
         <v>28</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>718</v>
+        <v>699</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>724</v>
+        <v>705</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>35</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>725</v>
+        <v>706</v>
       </c>
       <c r="R25" s="2" t="s">
         <v>35</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>726</v>
+        <v>707</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -5259,7 +5112,7 @@
         <v>139</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>727</v>
+        <v>708</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>21</v>
@@ -5288,10 +5141,10 @@
         <v>28</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>728</v>
+        <v>709</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>729</v>
+        <v>710</v>
       </c>
       <c r="P26" s="2" t="s">
         <v>35</v>
@@ -5303,7 +5156,7 @@
         <v>35</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>730</v>
+        <v>711</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -5314,7 +5167,7 @@
         <v>144</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>731</v>
+        <v>712</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>21</v>
@@ -5331,7 +5184,7 @@
         <v>145</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>92</v>
@@ -5343,10 +5196,10 @@
         <v>28</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>733</v>
+        <v>714</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>734</v>
+        <v>715</v>
       </c>
       <c r="P27" s="2" t="s">
         <v>35</v>
@@ -5369,7 +5222,7 @@
         <v>147</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>735</v>
+        <v>716</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>21</v>
@@ -5398,13 +5251,13 @@
         <v>28</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>736</v>
+        <v>717</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>737</v>
+        <v>718</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>738</v>
+        <v>719</v>
       </c>
       <c r="Q28" s="2" t="s">
         <v>35</v>
@@ -5424,7 +5277,7 @@
         <v>151</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>739</v>
+        <v>720</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>21</v>
@@ -5469,7 +5322,7 @@
         <v>154</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>740</v>
+        <v>721</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>21</v>
@@ -5524,7 +5377,7 @@
         <v>158</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>741</v>
+        <v>722</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>21</v>
@@ -5556,10 +5409,10 @@
         <v>35</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>742</v>
+        <v>723</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>743</v>
+        <v>724</v>
       </c>
       <c r="Q31" s="2" t="s">
         <v>35</v>
@@ -5579,7 +5432,7 @@
         <v>161</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>744</v>
+        <v>725</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>21</v>
@@ -5608,10 +5461,10 @@
         <v>28</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>745</v>
+        <v>726</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>746</v>
+        <v>727</v>
       </c>
       <c r="P32" s="2" t="s">
         <v>35</v>
@@ -5623,7 +5476,7 @@
         <v>35</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>747</v>
+        <v>728</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -5634,7 +5487,7 @@
         <v>167</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>748</v>
+        <v>729</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>21</v>
@@ -5679,7 +5532,7 @@
         <v>169</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>749</v>
+        <v>730</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>21</v>
@@ -5717,7 +5570,7 @@
         <v>35</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>750</v>
+        <v>731</v>
       </c>
       <c r="R34" s="2" t="s">
         <v>35</v>
@@ -5734,7 +5587,7 @@
         <v>173</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>751</v>
+        <v>732</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>21</v>
@@ -5789,7 +5642,7 @@
         <v>177</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>752</v>
+        <v>733</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>178</v>
@@ -5821,7 +5674,7 @@
         <v>184</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>753</v>
+        <v>734</v>
       </c>
       <c r="P36" s="2" t="s">
         <v>184</v>
@@ -5830,7 +5683,7 @@
         <v>184</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>754</v>
+        <v>735</v>
       </c>
       <c r="S36" s="2" t="s">
         <v>184</v>
@@ -5844,7 +5697,7 @@
         <v>186</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>755</v>
+        <v>736</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>178</v>
@@ -5877,16 +5730,16 @@
         <v>184</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>756</v>
+        <v>737</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>757</v>
+        <v>738</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>758</v>
+        <v>739</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>759</v>
+        <v>740</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -5897,7 +5750,7 @@
         <v>191</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>760</v>
+        <v>741</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>178</v>
@@ -5937,13 +5790,13 @@
         <v>184</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>761</v>
+        <v>742</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>762</v>
+        <v>743</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>763</v>
+        <v>744</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -5954,7 +5807,7 @@
         <v>196</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>764</v>
+        <v>745</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>178</v>
@@ -5986,13 +5839,13 @@
         <v>184</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>765</v>
+        <v>746</v>
       </c>
       <c r="P39" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>766</v>
+        <v>747</v>
       </c>
       <c r="R39" s="2" t="s">
         <v>184</v>
@@ -6009,7 +5862,7 @@
         <v>201</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>767</v>
+        <v>748</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>178</v>
@@ -6041,7 +5894,7 @@
         <v>184</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>768</v>
+        <v>749</v>
       </c>
       <c r="P40" s="2" t="s">
         <v>184</v>
@@ -6064,7 +5917,7 @@
         <v>206</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>769</v>
+        <v>750</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>178</v>
@@ -6093,7 +5946,7 @@
         <v>211</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>770</v>
+        <v>751</v>
       </c>
       <c r="O41" s="2" t="s">
         <v>212</v>
@@ -6119,7 +5972,7 @@
         <v>214</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>771</v>
+        <v>752</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>178</v>
@@ -6148,7 +6001,7 @@
         <v>28</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>772</v>
+        <v>753</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>184</v>
@@ -6160,10 +6013,10 @@
         <v>184</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>670</v>
+        <v>651</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>773</v>
+        <v>754</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -6174,7 +6027,7 @@
         <v>219</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>774</v>
+        <v>755</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>178</v>
@@ -6205,7 +6058,7 @@
         <v>28</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>775</v>
+        <v>756</v>
       </c>
       <c r="O43" s="2" t="s">
         <v>223</v>
@@ -6231,7 +6084,7 @@
         <v>225</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>776</v>
+        <v>757</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>178</v>
@@ -6260,7 +6113,7 @@
         <v>28</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>777</v>
+        <v>758</v>
       </c>
       <c r="O44" s="2" t="s">
         <v>184</v>
@@ -6272,10 +6125,10 @@
         <v>184</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>778</v>
+        <v>759</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>779</v>
+        <v>760</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -6286,7 +6139,7 @@
         <v>230</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>780</v>
+        <v>761</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>178</v>
@@ -6341,7 +6194,7 @@
         <v>235</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>781</v>
+        <v>762</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>236</v>
@@ -6360,28 +6213,28 @@
         <v>24</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>782</v>
+        <v>763</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>783</v>
+        <v>764</v>
       </c>
       <c r="M46" s="2" t="s">
         <v>239</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>770</v>
+        <v>751</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>650</v>
+        <v>631</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>618</v>
+        <v>599</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>784</v>
+        <v>765</v>
       </c>
       <c r="R46" s="2" t="s">
         <v>184</v>
@@ -6398,7 +6251,7 @@
         <v>241</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>785</v>
+        <v>766</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>236</v>
@@ -6417,7 +6270,7 @@
         <v>208</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>786</v>
+        <v>767</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>67</v>
@@ -6429,22 +6282,22 @@
         <v>28</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>787</v>
+        <v>768</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>788</v>
+        <v>769</v>
       </c>
       <c r="P47" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>789</v>
+        <v>770</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>790</v>
+        <v>771</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>791</v>
+        <v>772</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -6455,7 +6308,7 @@
         <v>244</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>792</v>
+        <v>773</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>236</v>
@@ -6472,7 +6325,7 @@
         <v>246</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>793</v>
+        <v>774</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>67</v>
@@ -6484,22 +6337,22 @@
         <v>28</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>794</v>
+        <v>775</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>795</v>
+        <v>776</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>796</v>
+        <v>777</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>797</v>
+        <v>778</v>
       </c>
       <c r="R48" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>798</v>
+        <v>779</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -6510,7 +6363,7 @@
         <v>249</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>799</v>
+        <v>780</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>236</v>
@@ -6539,22 +6392,22 @@
         <v>28</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>800</v>
+        <v>781</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>801</v>
+        <v>782</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>802</v>
+        <v>783</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>803</v>
+        <v>784</v>
       </c>
       <c r="R49" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>804</v>
+        <v>785</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -6565,7 +6418,7 @@
         <v>253</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>805</v>
+        <v>786</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>236</v>
@@ -6594,10 +6447,10 @@
         <v>28</v>
       </c>
       <c r="N50" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="O50" s="2" t="s">
         <v>787</v>
-      </c>
-      <c r="O50" s="2" t="s">
-        <v>806</v>
       </c>
       <c r="P50" s="2" t="s">
         <v>184</v>
@@ -6620,7 +6473,7 @@
         <v>256</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>807</v>
+        <v>788</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>236</v>
@@ -6647,22 +6500,22 @@
         <v>28</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>808</v>
+        <v>789</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>809</v>
+        <v>790</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>810</v>
+        <v>791</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>811</v>
+        <v>792</v>
       </c>
       <c r="R51" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>812</v>
+        <v>793</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
@@ -6673,7 +6526,7 @@
         <v>260</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>813</v>
+        <v>794</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>236</v>
@@ -6698,22 +6551,22 @@
         <v>33</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>783</v>
+        <v>764</v>
       </c>
       <c r="M52" s="2" t="s">
         <v>239</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>787</v>
+        <v>768</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>814</v>
+        <v>795</v>
       </c>
       <c r="P52" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>815</v>
+        <v>796</v>
       </c>
       <c r="R52" s="2" t="s">
         <v>184</v>
@@ -6730,7 +6583,7 @@
         <v>265</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>816</v>
+        <v>797</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>236</v>
@@ -6747,7 +6600,7 @@
         <v>46</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>817</v>
+        <v>798</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>92</v>
@@ -6759,10 +6612,10 @@
         <v>28</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>818</v>
+        <v>799</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>819</v>
+        <v>800</v>
       </c>
       <c r="P53" s="2" t="s">
         <v>184</v>
@@ -6774,7 +6627,7 @@
         <v>184</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>820</v>
+        <v>801</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
@@ -6785,7 +6638,7 @@
         <v>267</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>821</v>
+        <v>802</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>236</v>
@@ -6814,22 +6667,22 @@
         <v>28</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>822</v>
+        <v>803</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>823</v>
+        <v>804</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>824</v>
+        <v>805</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>825</v>
+        <v>806</v>
       </c>
       <c r="R54" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S54" s="2" t="s">
-        <v>826</v>
+        <v>807</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
@@ -6840,7 +6693,7 @@
         <v>271</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>827</v>
+        <v>808</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>236</v>
@@ -6869,10 +6722,10 @@
         <v>28</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>828</v>
+        <v>809</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>829</v>
+        <v>810</v>
       </c>
       <c r="P55" s="2" t="s">
         <v>184</v>
@@ -6881,10 +6734,10 @@
         <v>184</v>
       </c>
       <c r="R55" s="2" t="s">
-        <v>830</v>
+        <v>811</v>
       </c>
       <c r="S55" s="2" t="s">
-        <v>831</v>
+        <v>812</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
@@ -6895,7 +6748,7 @@
         <v>89</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>684</v>
+        <v>665</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>275</v>
@@ -6924,19 +6777,19 @@
         <v>28</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>832</v>
+        <v>813</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>833</v>
+        <v>814</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>834</v>
+        <v>815</v>
       </c>
       <c r="Q56" s="2" t="s">
         <v>184</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>835</v>
+        <v>816</v>
       </c>
       <c r="S56" s="2" t="s">
         <v>184</v>
@@ -6950,7 +6803,7 @@
         <v>161</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>744</v>
+        <v>725</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>275</v>
@@ -6967,7 +6820,7 @@
         <v>279</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>836</v>
+        <v>817</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>280</v>
@@ -6979,13 +6832,13 @@
         <v>28</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>837</v>
+        <v>818</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>838</v>
+        <v>819</v>
       </c>
       <c r="P57" s="2" t="s">
-        <v>839</v>
+        <v>820</v>
       </c>
       <c r="Q57" s="2" t="s">
         <v>184</v>
@@ -6994,7 +6847,7 @@
         <v>184</v>
       </c>
       <c r="S57" s="2" t="s">
-        <v>840</v>
+        <v>821</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
@@ -7005,7 +6858,7 @@
         <v>105</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>694</v>
+        <v>675</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>275</v>
@@ -7034,13 +6887,13 @@
         <v>28</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>841</v>
+        <v>822</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>842</v>
+        <v>823</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>843</v>
+        <v>824</v>
       </c>
       <c r="Q58" s="2" t="s">
         <v>184</v>
@@ -7060,7 +6913,7 @@
         <v>285</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>844</v>
+        <v>825</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>275</v>
@@ -7089,22 +6942,22 @@
         <v>28</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>845</v>
+        <v>826</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>846</v>
+        <v>827</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>847</v>
+        <v>828</v>
       </c>
       <c r="Q59" s="2" t="s">
-        <v>848</v>
+        <v>829</v>
       </c>
       <c r="R59" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S59" s="2" t="s">
-        <v>849</v>
+        <v>830</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
@@ -7115,7 +6968,7 @@
         <v>290</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>850</v>
+        <v>831</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>275</v>
@@ -7144,19 +6997,19 @@
         <v>28</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>851</v>
+        <v>832</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>852</v>
+        <v>833</v>
       </c>
       <c r="P60" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q60" s="2" t="s">
-        <v>853</v>
+        <v>834</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>854</v>
+        <v>835</v>
       </c>
       <c r="S60" s="2" t="s">
         <v>184</v>
@@ -7170,7 +7023,7 @@
         <v>294</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>855</v>
+        <v>836</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>275</v>
@@ -7189,7 +7042,7 @@
         <v>208</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>856</v>
+        <v>837</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>296</v>
@@ -7201,22 +7054,22 @@
         <v>28</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>857</v>
+        <v>838</v>
       </c>
       <c r="O61" s="2" t="s">
-        <v>858</v>
+        <v>839</v>
       </c>
       <c r="P61" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q61" s="2" t="s">
-        <v>859</v>
+        <v>840</v>
       </c>
       <c r="R61" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S61" s="2" t="s">
-        <v>860</v>
+        <v>841</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
@@ -7227,7 +7080,7 @@
         <v>298</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>861</v>
+        <v>842</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>275</v>
@@ -7256,13 +7109,13 @@
         <v>28</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>862</v>
+        <v>843</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>863</v>
+        <v>844</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>743</v>
+        <v>724</v>
       </c>
       <c r="Q62" s="2" t="s">
         <v>184</v>
@@ -7271,7 +7124,7 @@
         <v>184</v>
       </c>
       <c r="S62" s="2" t="s">
-        <v>730</v>
+        <v>711</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
@@ -7282,7 +7135,7 @@
         <v>302</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>864</v>
+        <v>845</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>275</v>
@@ -7311,19 +7164,19 @@
         <v>28</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>649</v>
+        <v>630</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>865</v>
+        <v>846</v>
       </c>
       <c r="P63" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q63" s="2" t="s">
-        <v>866</v>
+        <v>847</v>
       </c>
       <c r="R63" s="2" t="s">
-        <v>867</v>
+        <v>848</v>
       </c>
       <c r="S63" s="2" t="s">
         <v>184</v>
@@ -7337,7 +7190,7 @@
         <v>305</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>868</v>
+        <v>849</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>21</v>
@@ -7368,19 +7221,19 @@
         <v>28</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>869</v>
+        <v>850</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>870</v>
+        <v>851</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>871</v>
+        <v>852</v>
       </c>
       <c r="Q64" s="2" t="s">
         <v>184</v>
       </c>
       <c r="R64" s="2" t="s">
-        <v>872</v>
+        <v>853</v>
       </c>
       <c r="S64" s="2" t="s">
         <v>184</v>
@@ -7394,7 +7247,7 @@
         <v>311</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>873</v>
+        <v>854</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>21</v>
@@ -7425,22 +7278,22 @@
         <v>28</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>730</v>
+        <v>711</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>874</v>
+        <v>855</v>
       </c>
       <c r="P65" s="2" t="s">
-        <v>875</v>
+        <v>856</v>
       </c>
       <c r="Q65" s="2" t="s">
-        <v>876</v>
+        <v>857</v>
       </c>
       <c r="R65" s="2" t="s">
-        <v>682</v>
+        <v>663</v>
       </c>
       <c r="S65" s="2" t="s">
-        <v>877</v>
+        <v>858</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
@@ -7451,7 +7304,7 @@
         <v>315</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>878</v>
+        <v>859</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>316</v>
@@ -7470,7 +7323,7 @@
         <v>208</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>879</v>
+        <v>860</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>67</v>
@@ -7482,22 +7335,22 @@
         <v>320</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>880</v>
+        <v>861</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>881</v>
+        <v>862</v>
       </c>
       <c r="P66" s="2" t="s">
-        <v>882</v>
+        <v>863</v>
       </c>
       <c r="Q66" s="2" t="s">
-        <v>883</v>
+        <v>864</v>
       </c>
       <c r="R66" s="2" t="s">
-        <v>884</v>
+        <v>865</v>
       </c>
       <c r="S66" s="2" t="s">
-        <v>885</v>
+        <v>866</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
@@ -7508,7 +7361,7 @@
         <v>322</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>886</v>
+        <v>867</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>316</v>
@@ -7539,22 +7392,22 @@
         <v>327</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>887</v>
+        <v>868</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>888</v>
+        <v>869</v>
       </c>
       <c r="P67" s="2" t="s">
-        <v>889</v>
+        <v>870</v>
       </c>
       <c r="Q67" s="2" t="s">
         <v>184</v>
       </c>
       <c r="R67" s="2" t="s">
-        <v>890</v>
+        <v>871</v>
       </c>
       <c r="S67" s="2" t="s">
-        <v>891</v>
+        <v>872</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
@@ -7565,7 +7418,7 @@
         <v>329</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>892</v>
+        <v>873</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>316</v>
@@ -7598,18 +7451,18 @@
         <v>327</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>893</v>
+        <v>874</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>894</v>
+        <v>875</v>
       </c>
       <c r="P68" s="2"/>
       <c r="Q68" s="2" t="s">
-        <v>895</v>
+        <v>876</v>
       </c>
       <c r="R68" s="2"/>
       <c r="S68" s="2" t="s">
-        <v>896</v>
+        <v>877</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
@@ -7620,7 +7473,7 @@
         <v>336</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>897</v>
+        <v>878</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>316</v>
@@ -7653,10 +7506,10 @@
         <v>28</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>898</v>
+        <v>879</v>
       </c>
       <c r="O69" s="2" t="s">
-        <v>899</v>
+        <v>880</v>
       </c>
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
@@ -7671,7 +7524,7 @@
         <v>344</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>900</v>
+        <v>881</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>316</v>
@@ -7698,24 +7551,24 @@
         <v>67</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>783</v>
+        <v>764</v>
       </c>
       <c r="M70" s="2" t="s">
         <v>239</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>901</v>
+        <v>882</v>
       </c>
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
       <c r="Q70" s="2" t="s">
-        <v>902</v>
+        <v>883</v>
       </c>
       <c r="R70" s="2" t="s">
-        <v>903</v>
+        <v>884</v>
       </c>
       <c r="S70" s="2" t="s">
-        <v>904</v>
+        <v>885</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
@@ -7726,7 +7579,7 @@
         <v>350</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>905</v>
+        <v>886</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>316</v>
@@ -7757,20 +7610,20 @@
         <v>28</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>728</v>
+        <v>709</v>
       </c>
       <c r="O71" s="2" t="s">
-        <v>906</v>
+        <v>887</v>
       </c>
       <c r="P71" s="2" t="s">
-        <v>907</v>
+        <v>888</v>
       </c>
       <c r="Q71" s="2" t="s">
-        <v>908</v>
+        <v>889</v>
       </c>
       <c r="R71" s="2"/>
       <c r="S71" s="2" t="s">
-        <v>909</v>
+        <v>890</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
@@ -7781,7 +7634,7 @@
         <v>355</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>910</v>
+        <v>891</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>316</v>
@@ -7817,7 +7670,7 @@
         <v>184</v>
       </c>
       <c r="O72" s="2" t="s">
-        <v>911</v>
+        <v>892</v>
       </c>
       <c r="P72" s="2" t="s">
         <v>184</v>
@@ -7826,7 +7679,7 @@
         <v>184</v>
       </c>
       <c r="R72" s="2" t="s">
-        <v>912</v>
+        <v>893</v>
       </c>
       <c r="S72" s="2" t="s">
         <v>184</v>
@@ -7840,7 +7693,7 @@
         <v>361</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>913</v>
+        <v>894</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>316</v>
@@ -7867,7 +7720,7 @@
         <v>67</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>914</v>
+        <v>895</v>
       </c>
       <c r="M73" s="2" t="s">
         <v>320</v>
@@ -7876,7 +7729,7 @@
         <v>184</v>
       </c>
       <c r="O73" s="2" t="s">
-        <v>915</v>
+        <v>896</v>
       </c>
       <c r="P73" s="2" t="s">
         <v>184</v>
@@ -7885,7 +7738,7 @@
         <v>184</v>
       </c>
       <c r="R73" s="2" t="s">
-        <v>916</v>
+        <v>897</v>
       </c>
       <c r="S73" s="2" t="s">
         <v>184</v>
@@ -7899,7 +7752,7 @@
         <v>366</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>917</v>
+        <v>898</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>316</v>
@@ -7926,16 +7779,16 @@
         <v>369</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>918</v>
+        <v>899</v>
       </c>
       <c r="M74" s="2" t="s">
         <v>327</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>919</v>
+        <v>900</v>
       </c>
       <c r="O74" s="2" t="s">
-        <v>920</v>
+        <v>901</v>
       </c>
       <c r="P74" s="2" t="s">
         <v>184</v>
@@ -7944,7 +7797,7 @@
         <v>184</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>835</v>
+        <v>816</v>
       </c>
       <c r="S74" s="2" t="s">
         <v>184</v>
@@ -7958,7 +7811,7 @@
         <v>371</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>921</v>
+        <v>902</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>316</v>
@@ -7985,7 +7838,7 @@
         <v>67</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>922</v>
+        <v>903</v>
       </c>
       <c r="M75" s="2" t="s">
         <v>327</v>
@@ -8000,13 +7853,13 @@
         <v>184</v>
       </c>
       <c r="Q75" s="2" t="s">
-        <v>923</v>
+        <v>904</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>924</v>
+        <v>905</v>
       </c>
       <c r="S75" s="2" t="s">
-        <v>925</v>
+        <v>906</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
@@ -8017,7 +7870,7 @@
         <v>375</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>926</v>
+        <v>907</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>376</v>
@@ -8042,16 +7895,16 @@
         <v>67</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>914</v>
+        <v>895</v>
       </c>
       <c r="M76" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>927</v>
+        <v>908</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>928</v>
+        <v>909</v>
       </c>
       <c r="P76" s="2" t="s">
         <v>184</v>
@@ -8074,7 +7927,7 @@
         <v>382</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>929</v>
+        <v>910</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>376</v>
@@ -8110,7 +7963,7 @@
         <v>388</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>930</v>
+        <v>911</v>
       </c>
       <c r="P77" s="2" t="s">
         <v>184</v>
@@ -8133,7 +7986,7 @@
         <v>393</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>931</v>
+        <v>912</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>376</v>
@@ -8190,7 +8043,7 @@
         <v>400</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>932</v>
+        <v>913</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>376</v>
@@ -8221,13 +8074,13 @@
         <v>28</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>691</v>
+        <v>672</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>933</v>
+        <v>914</v>
       </c>
       <c r="P79" s="2" t="s">
-        <v>934</v>
+        <v>915</v>
       </c>
       <c r="Q79" s="2" t="s">
         <v>184</v>
@@ -8236,7 +8089,7 @@
         <v>184</v>
       </c>
       <c r="S79" s="2" t="s">
-        <v>935</v>
+        <v>916</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
@@ -8247,7 +8100,7 @@
         <v>404</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>936</v>
+        <v>917</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>376</v>
@@ -8288,7 +8141,7 @@
         <v>184</v>
       </c>
       <c r="R80" s="2" t="s">
-        <v>937</v>
+        <v>918</v>
       </c>
       <c r="S80" s="2" t="s">
         <v>184</v>
@@ -8302,7 +8155,7 @@
         <v>411</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>938</v>
+        <v>919</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>21</v>
@@ -8331,13 +8184,13 @@
         <v>28</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>862</v>
+        <v>843</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>939</v>
+        <v>920</v>
       </c>
       <c r="P81" s="2" t="s">
-        <v>940</v>
+        <v>921</v>
       </c>
       <c r="Q81" s="2" t="s">
         <v>184</v>
@@ -8357,7 +8210,7 @@
         <v>415</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>941</v>
+        <v>922</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>376</v>
@@ -8376,7 +8229,7 @@
         <v>24</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>942</v>
+        <v>923</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>33</v>
@@ -8388,13 +8241,13 @@
         <v>28</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>943</v>
+        <v>924</v>
       </c>
       <c r="O82" s="2" t="s">
-        <v>944</v>
+        <v>925</v>
       </c>
       <c r="P82" s="2" t="s">
-        <v>945</v>
+        <v>926</v>
       </c>
       <c r="Q82" s="2" t="s">
         <v>184</v>
@@ -8403,7 +8256,7 @@
         <v>184</v>
       </c>
       <c r="S82" s="2" t="s">
-        <v>946</v>
+        <v>927</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
@@ -8414,7 +8267,7 @@
         <v>419</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>947</v>
+        <v>928</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>376</v>
@@ -8443,16 +8296,16 @@
         <v>28</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>948</v>
+        <v>929</v>
       </c>
       <c r="O83" s="2" t="s">
-        <v>949</v>
+        <v>930</v>
       </c>
       <c r="P83" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q83" s="2" t="s">
-        <v>950</v>
+        <v>931</v>
       </c>
       <c r="R83" s="2" t="s">
         <v>184</v>
@@ -8469,7 +8322,7 @@
         <v>423</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>951</v>
+        <v>932</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>376</v>
@@ -8490,25 +8343,25 @@
         <v>24</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>615</v>
+        <v>596</v>
       </c>
       <c r="K84" s="2" t="s">
         <v>67</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>952</v>
+        <v>933</v>
       </c>
       <c r="M84" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>953</v>
+        <v>934</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>954</v>
+        <v>935</v>
       </c>
       <c r="P84" s="2" t="s">
-        <v>955</v>
+        <v>936</v>
       </c>
       <c r="Q84" s="2" t="s">
         <v>184</v>
@@ -8517,7 +8370,7 @@
         <v>184</v>
       </c>
       <c r="S84" s="2" t="s">
-        <v>956</v>
+        <v>937</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
@@ -8528,7 +8381,7 @@
         <v>427</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>957</v>
+        <v>938</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>376</v>
@@ -8557,13 +8410,13 @@
         <v>28</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>862</v>
+        <v>843</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>958</v>
+        <v>939</v>
       </c>
       <c r="P85" s="2" t="s">
-        <v>959</v>
+        <v>940</v>
       </c>
       <c r="Q85" s="2" t="s">
         <v>184</v>
@@ -8583,7 +8436,7 @@
         <v>432</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>960</v>
+        <v>941</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>433</v>
@@ -8613,10 +8466,10 @@
         <v>184</v>
       </c>
       <c r="O86" s="2" t="s">
-        <v>961</v>
+        <v>942</v>
       </c>
       <c r="P86" s="2" t="s">
-        <v>962</v>
+        <v>943</v>
       </c>
       <c r="Q86" s="2" t="s">
         <v>184</v>
@@ -8636,7 +8489,7 @@
         <v>344</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>900</v>
+        <v>881</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>433</v>
@@ -8665,22 +8518,22 @@
         <v>439</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>963</v>
+        <v>944</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>918</v>
+        <v>899</v>
       </c>
       <c r="P87" s="2" t="s">
-        <v>934</v>
+        <v>915</v>
       </c>
       <c r="Q87" s="2" t="s">
-        <v>964</v>
+        <v>945</v>
       </c>
       <c r="R87" s="2" t="s">
-        <v>965</v>
+        <v>946</v>
       </c>
       <c r="S87" s="2" t="s">
-        <v>966</v>
+        <v>947</v>
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
@@ -8691,7 +8544,7 @@
         <v>441</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>967</v>
+        <v>948</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>433</v>
@@ -8725,13 +8578,13 @@
         <v>184</v>
       </c>
       <c r="O88" s="2" t="s">
-        <v>968</v>
+        <v>949</v>
       </c>
       <c r="P88" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q88" s="2" t="s">
-        <v>969</v>
+        <v>950</v>
       </c>
       <c r="R88" s="2" t="s">
         <v>184</v>
@@ -8748,7 +8601,7 @@
         <v>446</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>970</v>
+        <v>951</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>433</v>
@@ -8767,7 +8620,7 @@
       </c>
       <c r="I89" s="2"/>
       <c r="J89" s="2" t="s">
-        <v>616</v>
+        <v>597</v>
       </c>
       <c r="K89" s="2" t="s">
         <v>67</v>
@@ -8777,10 +8630,10 @@
         <v>320</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>880</v>
+        <v>861</v>
       </c>
       <c r="O89" s="2" t="s">
-        <v>971</v>
+        <v>952</v>
       </c>
       <c r="P89" s="2" t="s">
         <v>184</v>
@@ -8789,10 +8642,10 @@
         <v>184</v>
       </c>
       <c r="R89" s="2" t="s">
-        <v>972</v>
+        <v>953</v>
       </c>
       <c r="S89" s="2" t="s">
-        <v>973</v>
+        <v>954</v>
       </c>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
@@ -8803,7 +8656,7 @@
         <v>441</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>967</v>
+        <v>948</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>433</v>
@@ -8835,13 +8688,13 @@
         <v>184</v>
       </c>
       <c r="O90" s="2" t="s">
-        <v>974</v>
+        <v>955</v>
       </c>
       <c r="P90" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>975</v>
+        <v>956</v>
       </c>
       <c r="R90" s="2" t="s">
         <v>184</v>
@@ -8858,7 +8711,7 @@
         <v>452</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>976</v>
+        <v>957</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>433</v>
@@ -8887,22 +8740,22 @@
         <v>28</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>977</v>
+        <v>958</v>
       </c>
       <c r="O91" s="2" t="s">
-        <v>978</v>
+        <v>959</v>
       </c>
       <c r="P91" s="2" t="s">
-        <v>979</v>
+        <v>960</v>
       </c>
       <c r="Q91" s="2" t="s">
-        <v>980</v>
+        <v>961</v>
       </c>
       <c r="R91" s="2" t="s">
-        <v>981</v>
+        <v>962</v>
       </c>
       <c r="S91" s="2" t="s">
-        <v>982</v>
+        <v>963</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
@@ -8913,7 +8766,7 @@
         <v>456</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>983</v>
+        <v>964</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>433</v>
@@ -8936,25 +8789,25 @@
         <v>67</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>914</v>
+        <v>895</v>
       </c>
       <c r="M92" s="2" t="s">
         <v>320</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>984</v>
+        <v>965</v>
       </c>
       <c r="O92" s="2" t="s">
-        <v>985</v>
+        <v>966</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>986</v>
+        <v>967</v>
       </c>
       <c r="Q92" s="2" t="s">
         <v>184</v>
       </c>
       <c r="R92" s="2" t="s">
-        <v>987</v>
+        <v>968</v>
       </c>
       <c r="S92" s="2" t="s">
         <v>184</v>
@@ -8968,7 +8821,7 @@
         <v>460</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>988</v>
+        <v>969</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>433</v>
@@ -8995,16 +8848,16 @@
         <v>320</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>989</v>
+        <v>970</v>
       </c>
       <c r="O93" s="2" t="s">
-        <v>990</v>
+        <v>971</v>
       </c>
       <c r="P93" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q93" s="2" t="s">
-        <v>991</v>
+        <v>972</v>
       </c>
       <c r="R93" s="2" t="s">
         <v>184</v>
@@ -9021,7 +8874,7 @@
         <v>464</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>992</v>
+        <v>973</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>433</v>
@@ -9046,28 +8899,28 @@
         <v>67</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>914</v>
+        <v>895</v>
       </c>
       <c r="M94" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>993</v>
+        <v>974</v>
       </c>
       <c r="O94" s="2" t="s">
-        <v>994</v>
+        <v>975</v>
       </c>
       <c r="P94" s="2" t="s">
-        <v>995</v>
+        <v>976</v>
       </c>
       <c r="Q94" s="2" t="s">
-        <v>996</v>
+        <v>977</v>
       </c>
       <c r="R94" s="2" t="s">
-        <v>997</v>
+        <v>978</v>
       </c>
       <c r="S94" s="2" t="s">
-        <v>998</v>
+        <v>979</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
@@ -9078,7 +8931,7 @@
         <v>393</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>931</v>
+        <v>912</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>433</v>
@@ -9099,7 +8952,7 @@
         <v>24</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>617</v>
+        <v>598</v>
       </c>
       <c r="K95" s="2" t="s">
         <v>67</v>
@@ -9135,7 +8988,7 @@
         <v>470</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>999</v>
+        <v>980</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>21</v>
@@ -9154,7 +9007,7 @@
         <v>46</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>618</v>
+        <v>599</v>
       </c>
       <c r="K96" s="2" t="s">
         <v>67</v>
@@ -9166,10 +9019,10 @@
         <v>28</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>1000</v>
+        <v>981</v>
       </c>
       <c r="O96" s="2" t="s">
-        <v>1001</v>
+        <v>982</v>
       </c>
       <c r="P96" s="2" t="s">
         <v>184</v>
@@ -9192,7 +9045,7 @@
         <v>473</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>1002</v>
+        <v>983</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>21</v>
@@ -9223,13 +9076,13 @@
         <v>28</v>
       </c>
       <c r="N97" s="2" t="s">
-        <v>733</v>
+        <v>714</v>
       </c>
       <c r="O97" s="2" t="s">
-        <v>1003</v>
+        <v>984</v>
       </c>
       <c r="P97" s="2" t="s">
-        <v>1004</v>
+        <v>985</v>
       </c>
       <c r="Q97" s="2" t="s">
         <v>184</v>
@@ -9249,7 +9102,7 @@
         <v>478</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>1005</v>
+        <v>986</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>21</v>
@@ -9280,10 +9133,10 @@
         <v>28</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>1006</v>
+        <v>987</v>
       </c>
       <c r="O98" s="2" t="s">
-        <v>895</v>
+        <v>876</v>
       </c>
       <c r="P98" s="2" t="s">
         <v>184</v>
@@ -9306,7 +9159,7 @@
         <v>375</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>926</v>
+        <v>907</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>21</v>
@@ -9337,10 +9190,10 @@
         <v>28</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>1007</v>
+        <v>988</v>
       </c>
       <c r="O99" s="2" t="s">
-        <v>1008</v>
+        <v>989</v>
       </c>
       <c r="P99" s="2" t="s">
         <v>184</v>
@@ -9363,7 +9216,7 @@
         <v>411</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>938</v>
+        <v>919</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>21</v>
@@ -9394,13 +9247,13 @@
         <v>28</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>1009</v>
+        <v>990</v>
       </c>
       <c r="O100" s="2" t="s">
-        <v>1010</v>
+        <v>991</v>
       </c>
       <c r="P100" s="2" t="s">
-        <v>1011</v>
+        <v>992</v>
       </c>
       <c r="Q100" s="2" t="s">
         <v>184</v>
@@ -9420,7 +9273,7 @@
         <v>486</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>1012</v>
+        <v>993</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>21</v>
@@ -9453,10 +9306,10 @@
         <v>28</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>1013</v>
+        <v>994</v>
       </c>
       <c r="O101" s="2" t="s">
-        <v>1014</v>
+        <v>995</v>
       </c>
       <c r="P101" s="2" t="s">
         <v>184</v>
@@ -9479,7 +9332,7 @@
         <v>371</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>921</v>
+        <v>902</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>21</v>
@@ -9519,13 +9372,13 @@
         <v>184</v>
       </c>
       <c r="Q102" s="2" t="s">
-        <v>1015</v>
+        <v>996</v>
       </c>
       <c r="R102" s="2" t="s">
-        <v>653</v>
+        <v>634</v>
       </c>
       <c r="S102" s="2" t="s">
-        <v>1016</v>
+        <v>997</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
@@ -9536,7 +9389,7 @@
         <v>494</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>1017</v>
+        <v>998</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>21</v>
@@ -9572,10 +9425,10 @@
         <v>184</v>
       </c>
       <c r="O103" s="2" t="s">
-        <v>1018</v>
+        <v>999</v>
       </c>
       <c r="P103" s="2" t="s">
-        <v>1019</v>
+        <v>1000</v>
       </c>
       <c r="Q103" s="2" t="s">
         <v>184</v>
@@ -9595,7 +9448,7 @@
         <v>415</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>941</v>
+        <v>922</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>21</v>
@@ -9626,13 +9479,13 @@
         <v>28</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>880</v>
+        <v>861</v>
       </c>
       <c r="O104" s="2" t="s">
-        <v>1020</v>
+        <v>1001</v>
       </c>
       <c r="P104" s="2" t="s">
-        <v>1021</v>
+        <v>1002</v>
       </c>
       <c r="Q104" s="2" t="s">
         <v>184</v>
@@ -9641,7 +9494,7 @@
         <v>184</v>
       </c>
       <c r="S104" s="2" t="s">
-        <v>1022</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
@@ -9652,7 +9505,7 @@
         <v>502</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>1023</v>
+        <v>1004</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>21</v>
@@ -9683,22 +9536,22 @@
         <v>28</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>1024</v>
+        <v>1005</v>
       </c>
       <c r="O105" s="2" t="s">
-        <v>1025</v>
+        <v>1006</v>
       </c>
       <c r="P105" s="2" t="s">
-        <v>1026</v>
+        <v>1007</v>
       </c>
       <c r="Q105" s="2" t="s">
-        <v>833</v>
+        <v>814</v>
       </c>
       <c r="R105" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S105" s="2" t="s">
-        <v>1027</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
@@ -9709,7 +9562,7 @@
         <v>508</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>1028</v>
+        <v>1009</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>509</v>
@@ -9738,22 +9591,22 @@
         <v>28</v>
       </c>
       <c r="N106" s="2" t="s">
-        <v>1029</v>
+        <v>1010</v>
       </c>
       <c r="O106" s="2" t="s">
-        <v>1030</v>
+        <v>1011</v>
       </c>
       <c r="P106" s="2" t="s">
-        <v>1031</v>
+        <v>1012</v>
       </c>
       <c r="Q106" s="2" t="s">
-        <v>1032</v>
+        <v>1013</v>
       </c>
       <c r="R106" s="2" t="s">
-        <v>912</v>
+        <v>893</v>
       </c>
       <c r="S106" s="2" t="s">
-        <v>1033</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
@@ -9764,7 +9617,7 @@
         <v>514</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>1034</v>
+        <v>1015</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>509</v>
@@ -9791,22 +9644,22 @@
         <v>239</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>1035</v>
+        <v>1016</v>
       </c>
       <c r="O107" s="2" t="s">
-        <v>1036</v>
+        <v>1017</v>
       </c>
       <c r="P107" s="2" t="s">
-        <v>1011</v>
+        <v>992</v>
       </c>
       <c r="Q107" s="2" t="s">
-        <v>1037</v>
+        <v>1018</v>
       </c>
       <c r="R107" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S107" s="2" t="s">
-        <v>1038</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
@@ -9817,7 +9670,7 @@
         <v>517</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>1039</v>
+        <v>1020</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>509</v>
@@ -9840,28 +9693,28 @@
         <v>33</v>
       </c>
       <c r="L108" s="2" t="s">
-        <v>1040</v>
+        <v>1021</v>
       </c>
       <c r="M108" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>1041</v>
+        <v>1022</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>1042</v>
+        <v>1023</v>
       </c>
       <c r="P108" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q108" s="2" t="s">
-        <v>1043</v>
+        <v>1024</v>
       </c>
       <c r="R108" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S108" s="2" t="s">
-        <v>826</v>
+        <v>807</v>
       </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
@@ -9872,7 +9725,7 @@
         <v>520</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>1044</v>
+        <v>1025</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>509</v>
@@ -9901,22 +9754,22 @@
         <v>28</v>
       </c>
       <c r="N109" s="2" t="s">
-        <v>1045</v>
+        <v>1026</v>
       </c>
       <c r="O109" s="2" t="s">
-        <v>1046</v>
+        <v>1027</v>
       </c>
       <c r="P109" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q109" s="2" t="s">
-        <v>1047</v>
+        <v>1028</v>
       </c>
       <c r="R109" s="2" t="s">
-        <v>867</v>
+        <v>848</v>
       </c>
       <c r="S109" s="2" t="s">
-        <v>1048</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
@@ -9927,7 +9780,7 @@
         <v>526</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>1049</v>
+        <v>1030</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>509</v>
@@ -9952,28 +9805,28 @@
         <v>33</v>
       </c>
       <c r="L110" s="2" t="s">
-        <v>1040</v>
+        <v>1021</v>
       </c>
       <c r="M110" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N110" s="2" t="s">
-        <v>1050</v>
+        <v>1031</v>
       </c>
       <c r="O110" s="2" t="s">
-        <v>1051</v>
+        <v>1032</v>
       </c>
       <c r="P110" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q110" s="2" t="s">
-        <v>1052</v>
+        <v>1033</v>
       </c>
       <c r="R110" s="2" t="s">
-        <v>1053</v>
+        <v>1034</v>
       </c>
       <c r="S110" s="2" t="s">
-        <v>1054</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
@@ -9984,7 +9837,7 @@
         <v>531</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>1055</v>
+        <v>1036</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>509</v>
@@ -10013,22 +9866,22 @@
         <v>28</v>
       </c>
       <c r="N111" s="2" t="s">
-        <v>1056</v>
+        <v>1037</v>
       </c>
       <c r="O111" s="2" t="s">
-        <v>1057</v>
+        <v>1038</v>
       </c>
       <c r="P111" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q111" s="2" t="s">
-        <v>1058</v>
+        <v>1039</v>
       </c>
       <c r="R111" s="2" t="s">
-        <v>1059</v>
+        <v>1040</v>
       </c>
       <c r="S111" s="2" t="s">
-        <v>1060</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
@@ -10039,7 +9892,7 @@
         <v>537</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>1061</v>
+        <v>1042</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>509</v>
@@ -10062,25 +9915,25 @@
         <v>67</v>
       </c>
       <c r="L112" s="2" t="s">
-        <v>1062</v>
+        <v>1043</v>
       </c>
       <c r="M112" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N112" s="2" t="s">
-        <v>1063</v>
+        <v>1044</v>
       </c>
       <c r="O112" s="2" t="s">
-        <v>1064</v>
+        <v>1045</v>
       </c>
       <c r="P112" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q112" s="2" t="s">
-        <v>1065</v>
+        <v>1046</v>
       </c>
       <c r="R112" s="2" t="s">
-        <v>1066</v>
+        <v>1047</v>
       </c>
       <c r="S112" s="2" t="s">
         <v>184</v>
@@ -10094,7 +9947,7 @@
         <v>541</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>1067</v>
+        <v>1048</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>509</v>
@@ -10119,28 +9972,28 @@
         <v>33</v>
       </c>
       <c r="L113" s="2" t="s">
-        <v>1051</v>
+        <v>1032</v>
       </c>
       <c r="M113" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>1068</v>
+        <v>1049</v>
       </c>
       <c r="O113" s="2" t="s">
-        <v>1069</v>
+        <v>1050</v>
       </c>
       <c r="P113" s="2" t="s">
-        <v>1070</v>
+        <v>1051</v>
       </c>
       <c r="Q113" s="2" t="s">
-        <v>1071</v>
+        <v>1052</v>
       </c>
       <c r="R113" s="2" t="s">
-        <v>1072</v>
+        <v>1053</v>
       </c>
       <c r="S113" s="2" t="s">
-        <v>1073</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
@@ -10151,7 +10004,7 @@
         <v>544</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>1074</v>
+        <v>1055</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>509</v>
@@ -10184,10 +10037,10 @@
         <v>28</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>1075</v>
+        <v>1056</v>
       </c>
       <c r="O114" s="2" t="s">
-        <v>1076</v>
+        <v>1057</v>
       </c>
       <c r="P114" s="2" t="s">
         <v>184</v>
@@ -10196,7 +10049,7 @@
         <v>184</v>
       </c>
       <c r="R114" s="2" t="s">
-        <v>1077</v>
+        <v>1058</v>
       </c>
       <c r="S114" s="2" t="s">
         <v>184</v>
@@ -10210,7 +10063,7 @@
         <v>550</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>1078</v>
+        <v>1059</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>509</v>
@@ -10237,22 +10090,22 @@
         <v>28</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>1079</v>
+        <v>1060</v>
       </c>
       <c r="O115" s="2" t="s">
-        <v>1080</v>
+        <v>1061</v>
       </c>
       <c r="P115" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q115" s="2" t="s">
-        <v>949</v>
+        <v>930</v>
       </c>
       <c r="R115" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S115" s="2" t="s">
-        <v>1081</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
@@ -10263,7 +10116,7 @@
         <v>556</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>1082</v>
+        <v>1063</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>21</v>
@@ -10294,7 +10147,7 @@
         <v>28</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>1029</v>
+        <v>1010</v>
       </c>
       <c r="O116" s="2" t="s">
         <v>184</v>
@@ -10303,13 +10156,13 @@
         <v>184</v>
       </c>
       <c r="Q116" s="2" t="s">
-        <v>696</v>
+        <v>677</v>
       </c>
       <c r="R116" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S116" s="2" t="s">
-        <v>1083</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
@@ -10320,7 +10173,7 @@
         <v>560</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>1084</v>
+        <v>1065</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>21</v>
@@ -10354,13 +10207,13 @@
         <v>184</v>
       </c>
       <c r="O117" s="2" t="s">
-        <v>1085</v>
+        <v>1066</v>
       </c>
       <c r="P117" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q117" s="2" t="s">
-        <v>1086</v>
+        <v>1067</v>
       </c>
       <c r="R117" s="2" t="s">
         <v>184</v>
@@ -10377,7 +10230,7 @@
         <v>566</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>1087</v>
+        <v>1068</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>21</v>
@@ -10404,22 +10257,22 @@
         <v>239</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>1088</v>
+        <v>1069</v>
       </c>
       <c r="O118" s="2" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="P118" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q118" s="2" t="s">
-        <v>1089</v>
+        <v>1070</v>
       </c>
       <c r="R118" s="2" t="s">
-        <v>924</v>
+        <v>905</v>
       </c>
       <c r="S118" s="2" t="s">
-        <v>1090</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
@@ -10430,7 +10283,7 @@
         <v>569</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>1091</v>
+        <v>1072</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>21</v>
@@ -10461,22 +10314,22 @@
         <v>28</v>
       </c>
       <c r="N119" s="2" t="s">
-        <v>822</v>
+        <v>803</v>
       </c>
       <c r="O119" s="2" t="s">
-        <v>1092</v>
+        <v>1073</v>
       </c>
       <c r="P119" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q119" s="2" t="s">
-        <v>1093</v>
+        <v>1074</v>
       </c>
       <c r="R119" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S119" s="2" t="s">
-        <v>1094</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
@@ -10487,7 +10340,7 @@
         <v>573</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>1095</v>
+        <v>1076</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>21</v>
@@ -10518,10 +10371,10 @@
         <v>28</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>1096</v>
+        <v>1077</v>
       </c>
       <c r="O120" s="2" t="s">
-        <v>1097</v>
+        <v>1078</v>
       </c>
       <c r="P120" s="2" t="s">
         <v>184</v>
@@ -10544,7 +10397,7 @@
         <v>580</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>1098</v>
+        <v>1079</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>21</v>
@@ -10561,7 +10414,7 @@
       </c>
       <c r="I121" s="2"/>
       <c r="J121" s="2" t="s">
-        <v>1099</v>
+        <v>1080</v>
       </c>
       <c r="K121" s="2" t="s">
         <v>33</v>
@@ -10573,10 +10426,10 @@
         <v>28</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>1100</v>
+        <v>1081</v>
       </c>
       <c r="O121" s="2" t="s">
-        <v>1101</v>
+        <v>1082</v>
       </c>
       <c r="P121" s="2" t="s">
         <v>184</v>
@@ -10588,7 +10441,7 @@
         <v>184</v>
       </c>
       <c r="S121" s="2" t="s">
-        <v>1102</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
@@ -10599,7 +10452,7 @@
         <v>584</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>1103</v>
+        <v>1084</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>21</v>
@@ -10614,7 +10467,7 @@
       </c>
       <c r="I122" s="2"/>
       <c r="J122" s="2" t="s">
-        <v>614</v>
+        <v>595</v>
       </c>
       <c r="K122" s="2" t="s">
         <v>67</v>
@@ -10650,7 +10503,7 @@
         <v>586</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>1104</v>
+        <v>1085</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>21</v>
@@ -10697,7 +10550,7 @@
         <v>588</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>1105</v>
+        <v>1086</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>21</v>
@@ -10744,7 +10597,7 @@
         <v>569</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>1091</v>
+        <v>1072</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>21</v>
@@ -10773,22 +10626,22 @@
         <v>28</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>1106</v>
+        <v>1087</v>
       </c>
       <c r="O125" s="2" t="s">
-        <v>1107</v>
+        <v>1088</v>
       </c>
       <c r="P125" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q125" s="2" t="s">
-        <v>1108</v>
+        <v>1089</v>
       </c>
       <c r="R125" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S125" s="2" t="s">
-        <v>1109</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
@@ -10799,7 +10652,7 @@
         <v>544</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>1074</v>
+        <v>1055</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>21</v>
@@ -10828,10 +10681,10 @@
         <v>28</v>
       </c>
       <c r="N126" s="2" t="s">
-        <v>1110</v>
+        <v>1091</v>
       </c>
       <c r="O126" s="2" t="s">
-        <v>1111</v>
+        <v>1092</v>
       </c>
       <c r="P126" s="2" t="s">
         <v>184</v>
@@ -10840,7 +10693,7 @@
         <v>184</v>
       </c>
       <c r="R126" s="2" t="s">
-        <v>1112</v>
+        <v>1093</v>
       </c>
       <c r="S126" s="2" t="s">
         <v>184</v>
@@ -10854,7 +10707,7 @@
         <v>541</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>1067</v>
+        <v>1048</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>21</v>
@@ -10877,28 +10730,28 @@
         <v>33</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>1051</v>
+        <v>1032</v>
       </c>
       <c r="M127" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N127" s="2" t="s">
-        <v>1113</v>
+        <v>1094</v>
       </c>
       <c r="O127" s="2" t="s">
-        <v>721</v>
+        <v>702</v>
       </c>
       <c r="P127" s="2" t="s">
-        <v>1114</v>
+        <v>1095</v>
       </c>
       <c r="Q127" s="2" t="s">
-        <v>1115</v>
+        <v>1096</v>
       </c>
       <c r="R127" s="2" t="s">
-        <v>1053</v>
+        <v>1034</v>
       </c>
       <c r="S127" s="2" t="s">
-        <v>1116</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
@@ -10909,7 +10762,7 @@
         <v>537</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>1061</v>
+        <v>1042</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>21</v>
@@ -10932,22 +10785,22 @@
         <v>67</v>
       </c>
       <c r="L128" s="2" t="s">
-        <v>1062</v>
+        <v>1043</v>
       </c>
       <c r="M128" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N128" s="2" t="s">
-        <v>745</v>
+        <v>726</v>
       </c>
       <c r="O128" s="2" t="s">
-        <v>1117</v>
+        <v>1098</v>
       </c>
       <c r="P128" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q128" s="2" t="s">
-        <v>1118</v>
+        <v>1099</v>
       </c>
       <c r="R128" s="2" t="s">
         <v>184</v>
@@ -10964,7 +10817,7 @@
         <v>400</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>932</v>
+        <v>913</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>21</v>
@@ -10995,13 +10848,13 @@
         <v>28</v>
       </c>
       <c r="N129" s="2" t="s">
-        <v>1119</v>
+        <v>1100</v>
       </c>
       <c r="O129" s="2" t="s">
-        <v>1120</v>
+        <v>1101</v>
       </c>
       <c r="P129" s="2" t="s">
-        <v>1121</v>
+        <v>1102</v>
       </c>
       <c r="Q129" s="2" t="s">
         <v>184</v>
@@ -11010,7 +10863,7 @@
         <v>184</v>
       </c>
       <c r="S129" s="2" t="s">
-        <v>1122</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
@@ -11021,7 +10874,7 @@
         <v>441</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>967</v>
+        <v>948</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>21</v>
@@ -11053,13 +10906,13 @@
         <v>184</v>
       </c>
       <c r="O130" s="2" t="s">
-        <v>1123</v>
+        <v>1104</v>
       </c>
       <c r="P130" s="2" t="s">
         <v>184</v>
       </c>
       <c r="Q130" s="2" t="s">
-        <v>1124</v>
+        <v>1105</v>
       </c>
       <c r="R130" s="2" t="s">
         <v>184</v>
@@ -11070,15 +10923,17 @@
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>593</v>
+        <v>321</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>594</v>
+        <v>322</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>1125</v>
-      </c>
-      <c r="D131" s="2"/>
+        <v>867</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>316</v>
+      </c>
       <c r="E131" s="2"/>
       <c r="F131" s="2" t="s">
         <v>591</v>
@@ -11087,504 +10942,148 @@
       <c r="H131" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="I131" s="2"/>
-      <c r="J131" s="2"/>
+      <c r="I131" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J131" s="2" t="s">
+        <v>593</v>
+      </c>
       <c r="K131" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="L131" s="2"/>
-      <c r="M131" s="2"/>
+      <c r="L131" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="M131" s="2" t="s">
+        <v>327</v>
+      </c>
       <c r="N131" s="2" t="s">
-        <v>1126</v>
+        <v>1106</v>
       </c>
       <c r="O131" s="2" t="s">
-        <v>1127</v>
+        <v>1107</v>
       </c>
       <c r="P131" s="2" t="s">
-        <v>1128</v>
+        <v>1108</v>
       </c>
       <c r="Q131" s="2" t="s">
-        <v>1129</v>
+        <v>184</v>
       </c>
       <c r="R131" s="2" t="s">
-        <v>184</v>
+        <v>1109</v>
       </c>
       <c r="S131" s="2" t="s">
-        <v>1130</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>595</v>
+        <v>304</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>596</v>
+        <v>305</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D132" s="2"/>
+        <v>849</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="E132" s="2"/>
       <c r="F132" s="2" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="G132" s="2"/>
       <c r="H132" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I132" s="2"/>
-      <c r="J132" s="2"/>
+        <v>180</v>
+      </c>
+      <c r="I132" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>308</v>
+      </c>
       <c r="K132" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="L132" s="2"/>
-      <c r="M132" s="2"/>
+      <c r="L132" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="M132" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="N132" s="2" t="s">
-        <v>1132</v>
+        <v>184</v>
       </c>
       <c r="O132" s="2" t="s">
-        <v>1133</v>
+        <v>1111</v>
       </c>
       <c r="P132" s="2" t="s">
-        <v>1134</v>
+        <v>1112</v>
       </c>
       <c r="Q132" s="2" t="s">
-        <v>1135</v>
+        <v>184</v>
       </c>
       <c r="R132" s="2" t="s">
-        <v>184</v>
+        <v>1113</v>
       </c>
       <c r="S132" s="2" t="s">
-        <v>763</v>
+        <v>184</v>
       </c>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>597</v>
+        <v>284</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>598</v>
+        <v>285</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>1136</v>
-      </c>
-      <c r="D133" s="2"/>
+        <v>825</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="E133" s="2"/>
       <c r="F133" s="2" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="G133" s="2"/>
       <c r="H133" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="I133" s="2"/>
-      <c r="J133" s="2"/>
-      <c r="K133" s="2"/>
-      <c r="L133" s="2"/>
-      <c r="M133" s="2"/>
+        <v>207</v>
+      </c>
+      <c r="I133" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="K133" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L133" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="M133" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="N133" s="2" t="s">
-        <v>184</v>
+        <v>744</v>
       </c>
       <c r="O133" s="2" t="s">
-        <v>184</v>
+        <v>1114</v>
       </c>
       <c r="P133" s="2" t="s">
-        <v>184</v>
+        <v>724</v>
       </c>
       <c r="Q133" s="2" t="s">
-        <v>184</v>
+        <v>796</v>
       </c>
       <c r="R133" s="2" t="s">
         <v>184</v>
       </c>
       <c r="S133" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>886</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="E134" s="2"/>
-      <c r="F134" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="G134" s="2"/>
-      <c r="H134" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="I134" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="J134" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="K134" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L134" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="M134" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="N134" s="2" t="s">
-        <v>1137</v>
-      </c>
-      <c r="O134" s="2" t="s">
-        <v>1138</v>
-      </c>
-      <c r="P134" s="2" t="s">
-        <v>1139</v>
-      </c>
-      <c r="Q134" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="R134" s="2" t="s">
-        <v>1140</v>
-      </c>
-      <c r="S134" s="2" t="s">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>1142</v>
-      </c>
-      <c r="D135" s="2"/>
-      <c r="E135" s="2"/>
-      <c r="F135" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="G135" s="2"/>
-      <c r="H135" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="I135" s="2"/>
-      <c r="J135" s="2"/>
-      <c r="K135" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L135" s="2"/>
-      <c r="M135" s="2"/>
-      <c r="N135" s="2" t="s">
-        <v>1143</v>
-      </c>
-      <c r="O135" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="P135" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q135" s="2" t="s">
-        <v>1144</v>
-      </c>
-      <c r="R135" s="2" t="s">
-        <v>1072</v>
-      </c>
-      <c r="S135" s="2" t="s">
-        <v>1145</v>
-      </c>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>1146</v>
-      </c>
-      <c r="D136" s="2"/>
-      <c r="E136" s="2"/>
-      <c r="F136" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="G136" s="2"/>
-      <c r="H136" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I136" s="2"/>
-      <c r="J136" s="2"/>
-      <c r="K136" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L136" s="2"/>
-      <c r="M136" s="2"/>
-      <c r="N136" s="2" t="s">
-        <v>1147</v>
-      </c>
-      <c r="O136" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="P136" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q136" s="2" t="s">
-        <v>1093</v>
-      </c>
-      <c r="R136" s="2" t="s">
-        <v>867</v>
-      </c>
-      <c r="S136" s="2" t="s">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>1149</v>
-      </c>
-      <c r="D137" s="2"/>
-      <c r="E137" s="2"/>
-      <c r="F137" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="G137" s="2"/>
-      <c r="H137" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I137" s="2"/>
-      <c r="J137" s="2"/>
-      <c r="K137" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L137" s="2"/>
-      <c r="M137" s="2"/>
-      <c r="N137" s="2" t="s">
-        <v>1150</v>
-      </c>
-      <c r="O137" s="2" t="s">
-        <v>1151</v>
-      </c>
-      <c r="P137" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q137" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="R137" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="S137" s="2" t="s">
-        <v>1152</v>
-      </c>
-    </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>1153</v>
-      </c>
-      <c r="D138" s="2"/>
-      <c r="E138" s="2"/>
-      <c r="F138" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="G138" s="2"/>
-      <c r="H138" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I138" s="2"/>
-      <c r="J138" s="2"/>
-      <c r="K138" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="L138" s="2"/>
-      <c r="M138" s="2"/>
-      <c r="N138" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="O138" s="2" t="s">
-        <v>1154</v>
-      </c>
-      <c r="P138" s="2" t="s">
-        <v>1155</v>
-      </c>
-      <c r="Q138" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="R138" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="S138" s="2" t="s">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>1153</v>
-      </c>
-      <c r="D139" s="2"/>
-      <c r="E139" s="2"/>
-      <c r="F139" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="G139" s="2"/>
-      <c r="H139" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I139" s="2"/>
-      <c r="J139" s="2"/>
-      <c r="K139" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="L139" s="2"/>
-      <c r="M139" s="2"/>
-      <c r="N139" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="O139" s="2" t="s">
-        <v>1157</v>
-      </c>
-      <c r="P139" s="2" t="s">
-        <v>1158</v>
-      </c>
-      <c r="Q139" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="R139" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="S139" s="2" t="s">
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>868</v>
-      </c>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="G140" s="2"/>
-      <c r="H140" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="I140" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="J140" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="K140" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L140" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="M140" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N140" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="O140" s="2" t="s">
-        <v>1160</v>
-      </c>
-      <c r="P140" s="2" t="s">
-        <v>1161</v>
-      </c>
-      <c r="Q140" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="R140" s="2" t="s">
-        <v>1162</v>
-      </c>
-      <c r="S140" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="G141" s="2"/>
-      <c r="H141" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I141" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="J141" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="K141" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L141" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="M141" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N141" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="O141" s="2" t="s">
-        <v>1163</v>
-      </c>
-      <c r="P141" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="Q141" s="2" t="s">
-        <v>815</v>
-      </c>
-      <c r="R141" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="S141" s="2" t="s">
-        <v>1164</v>
+        <v>1115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>